<commit_message>
Prep for adding submodules frame designed
</commit_message>
<xml_diff>
--- a/frameSpecifications.xlsx
+++ b/frameSpecifications.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\Models\Four Paddle Detector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\muonTelescope\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>height</t>
   </si>
   <si>
-    <t>cm</t>
-  </si>
-  <si>
     <t>width</t>
   </si>
   <si>
@@ -41,7 +38,13 @@
     <t>botSeparation</t>
   </si>
   <si>
-    <t>panelChamfer</t>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>suppourtPanelThickness</t>
+  </si>
+  <si>
+    <t>in</t>
   </si>
 </sst>
 </file>
@@ -172,6 +175,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -207,6 +227,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -362,7 +399,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,43 +412,43 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -419,13 +456,14 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>7.5</v>
+        <v>9.375E-2</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>